<commit_message>
Clean up and fix unit tests. Fix worksheet names for xlsx Fix formatting for xlsx. Add github action to build and test.
</commit_message>
<xml_diff>
--- a/source/Sylvan.Data.Excel.Tests/Data/Xlsx/func.xlsx
+++ b/source/Sylvan.Data.Excel.Tests/Data/Xlsx/func.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\source\Sylvan.Data.Excel\source\Sylvan.Data.Excel.Tests\Data\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250368BE-3E40-4068-8150-4B856E80FCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C54B2BAE-99E8-46F2-BF30-E34958A6D14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4560" windowWidth="21600" windowHeight="12735" xr2:uid="{4825C0CE-CE27-4FB3-B301-19DAE0548D60}"/>
+    <workbookView xWindow="2610" yWindow="2220" windowWidth="21600" windowHeight="12735"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,19 +86,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="OTHER"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,11 +384,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E7B47E-9F04-4E0E-A33B-99509E7908FC}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +398,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="b">
-        <f t="shared" ref="B1:B5" si="0">MOD(A1,2)=0</f>
+        <f>MOD(A1,2)=0</f>
         <v>1</v>
       </c>
       <c r="C1" t="e">
@@ -424,11 +411,11 @@
         <v>1</v>
       </c>
       <c r="B2" t="b">
-        <f t="shared" si="0"/>
+        <f>MOD(A2,2)=0</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C5" si="1">A3/A2</f>
+        <f>A3/A2</f>
         <v>2</v>
       </c>
     </row>
@@ -441,7 +428,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="1"/>
+        <f>A4/A3</f>
         <v>1.5</v>
       </c>
     </row>
@@ -450,11 +437,11 @@
         <v>3</v>
       </c>
       <c r="B4" t="b">
-        <f t="shared" si="0"/>
+        <f>MOD(A4,2)=0</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f>A5/A4</f>
         <v>2</v>
       </c>
     </row>
@@ -464,11 +451,11 @@
         <v>6</v>
       </c>
       <c r="B5" t="b">
-        <f t="shared" si="0"/>
+        <f>MOD(A5,2)=0</f>
         <v>1</v>
       </c>
       <c r="C5" t="e">
-        <f t="shared" si="1"/>
+        <f>A6/A5</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -482,24 +469,6 @@
       <c r="C6" t="str">
         <f>A6&amp;B6</f>
         <v>ab</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="e">
-        <f>[1]OTHER!A1</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="e">
-        <f ca="1">Vlocup(A1:B3)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="e">
-        <f>SUM(A1 B1)</f>
-        <v>#NULL!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>